<commit_message>
conversion of few-nerd data
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callum\OneDrive\MSc datascience\DSM 500 final project\Fine grained entity tagging with large language models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D79B3B3-410A-4BFB-9C54-098DAFCBAD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AEC129-72A2-4AB1-878C-903547D9FF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="2" r:id="rId1"/>
-    <sheet name="Ideas" sheetId="1" r:id="rId2"/>
-    <sheet name="Diary" sheetId="3" r:id="rId3"/>
-    <sheet name="Project Plan" sheetId="5" r:id="rId4"/>
+    <sheet name="gant chart" sheetId="6" r:id="rId2"/>
+    <sheet name="Ideas" sheetId="1" r:id="rId3"/>
+    <sheet name="Diary" sheetId="3" r:id="rId4"/>
     <sheet name="Work Record" sheetId="4" r:id="rId5"/>
+    <sheet name="Project Plan - proposal" sheetId="5" r:id="rId6"/>
+    <sheet name="project plan - project" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Project Plan'!$A$3:$D$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Project Plan - proposal'!$A$3:$D$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="129">
   <si>
     <t>Ideas</t>
   </si>
@@ -159,9 +161,6 @@
   </si>
   <si>
     <t>Complete</t>
-  </si>
-  <si>
-    <t>Not Started</t>
   </si>
   <si>
     <t>Idea ID</t>
@@ -571,6 +570,57 @@
     <t>sent off a proposal idea to supervisor.
  Read about how prompt engineering is being used in FGET and LLMs in general in NET.
 Updated the project plan for weeks 7/8/9</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>start date</t>
+  </si>
+  <si>
+    <t>days to complete</t>
+  </si>
+  <si>
+    <t>holiday</t>
+  </si>
+  <si>
+    <t>Project writeup</t>
+  </si>
+  <si>
+    <t>sub-tasks</t>
+  </si>
+  <si>
+    <t>end date</t>
+  </si>
+  <si>
+    <t>expected end date</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>6.1 - prepare BERT and Few-Nerd dataset</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>get Few-nerd dataset into a format that is reasonable for BERT</t>
+  </si>
+  <si>
+    <t>Get Bert downloaded from hugging face and ensure it works.</t>
+  </si>
+  <si>
+    <t>not started</t>
+  </si>
+  <si>
+    <t>6.0 - report write up</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>literature review</t>
   </si>
 </sst>
 </file>
@@ -633,7 +683,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -682,12 +732,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -704,6 +795,23 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -763,6 +871,1140 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Project Plan Timeline</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'gant chart'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>start date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'gant chart'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>holiday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Project writeup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'gant chart'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45117</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45171</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45110</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCC2-4050-834D-F2FE2A91A45B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'gant chart'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>days to complete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="pct90">
+                <a:fgClr>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-FCC2-4050-834D-F2FE2A91A45B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'gant chart'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>holiday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Project writeup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'gant chart'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FCC2-4050-834D-F2FE2A91A45B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="95"/>
+        <c:overlap val="100"/>
+        <c:axId val="643513976"/>
+        <c:axId val="643514336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="643513976"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="643514336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="643514336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="45105"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="643513976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:softEdge rad="0"/>
+        </a:effectLst>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1240E414-BDB4-FAA8-3207-772F901F5C8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1030,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B28A28D-17E8-483A-800B-C8F9D71918C5}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +2291,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1078,22 +2320,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="405" x14ac:dyDescent="0.25">
@@ -1104,22 +2346,22 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1130,22 +2372,22 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1156,22 +2398,22 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="H5" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1182,22 +2424,22 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1208,13 +2450,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1225,13 +2467,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1242,22 +2484,22 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1268,22 +2510,22 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1294,22 +2536,22 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1319,13 +2561,134 @@
     <hyperlink ref="H8" r:id="rId3" xr:uid="{88F1C3B4-BDD9-4CBF-ABC6-39F33C45BD1B}"/>
     <hyperlink ref="H9" r:id="rId4" xr:uid="{1FEA3B93-0A2E-4126-B53A-99B72F077AE3}"/>
     <hyperlink ref="H10" r:id="rId5" xr:uid="{A3BDDD5A-CB1C-416D-BC3F-E01F3CD67B58}"/>
+    <hyperlink ref="H11" r:id="rId6" xr:uid="{692CD3C6-8367-40C9-9525-F262583E7553}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE931ECE-F2F0-4798-9EDF-78880E6A2CA1}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6.1</v>
+      </c>
+      <c r="B2" s="13">
+        <v>45103</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="13">
+        <v>45110</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6.2</v>
+      </c>
+      <c r="B4" s="13">
+        <v>45117</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>45129</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6.4</v>
+      </c>
+      <c r="B6" s="13">
+        <v>45150</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.5</v>
+      </c>
+      <c r="B7" s="13">
+        <v>45171</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="13">
+        <v>45110</v>
+      </c>
+      <c r="C8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
+        <v>45133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
@@ -1340,7 +2703,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1379,7 +2742,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -1387,17 +2750,17 @@
         <v>3</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
@@ -1408,7 +2771,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
@@ -1419,7 +2782,7 @@
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
@@ -1430,7 +2793,7 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
@@ -1441,7 +2804,7 @@
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
@@ -1455,7 +2818,7 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
@@ -1463,37 +2826,37 @@
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
@@ -1501,7 +2864,7 @@
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +2873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41132F2D-8B63-45FB-A93C-B3FE579EE3F6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1524,13 +2887,110 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E69907-D83B-4E58-94C9-1AF9892C2EF0}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45040</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45041</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45042</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45066</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45076</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>45082</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8764B460-41FE-40A4-B365-EE26B632B85C}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +3014,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">WEEKNUM(TODAY()) -WEEKNUM(B1) +1</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1612,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
@@ -1623,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -1637,7 +3097,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,7 +3119,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1667,7 +3130,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,7 +3141,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1683,7 +3152,15 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1729,99 +3206,114 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E69907-D83B-4E58-94C9-1AF9892C2EF0}">
-  <dimension ref="A1:C7"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E288C7F7-F28B-4777-96A5-B7B72B96D9FC}">
+  <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>45040</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45041</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>45042</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>45066</v>
-      </c>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>45076</v>
-      </c>
-      <c r="B6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>45082</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15">
+        <v>45185</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="15">
+        <v>45123</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="18">
+        <v>45123</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="15">
+        <v>45123</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="14" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A3:A4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>